<commit_message>
Sorting files for better organization
</commit_message>
<xml_diff>
--- a/Spreadsheet/FromLB/20190227 LDB to LEMIR E_I_Mapping Sharon 2nd update.xlsx
+++ b/Spreadsheet/FromLB/20190227 LDB to LEMIR E_I_Mapping Sharon 2nd update.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\Solid Waste Migration\Spreadsheet\FromLB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\Spreadsheet\FromLB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652E636D-DC1C-40CA-8BDF-E3569183C17D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE19B73-CDA1-41B3-9EF2-126A548BAA25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="636" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -7334,25 +7334,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" style="22" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="54.28515625" customWidth="1"/>
-    <col min="11" max="11" width="37.42578125" customWidth="1"/>
+    <col min="6" max="6" width="38.88671875" style="22" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="54.33203125" customWidth="1"/>
+    <col min="11" max="11" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="67" t="s">
         <v>110</v>
       </c>
@@ -7368,7 +7368,7 @@
       <c r="J1" s="67"/>
       <c r="K1" s="67"/>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>109</v>
       </c>
@@ -7400,7 +7400,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>72</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>24</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>83</v>
       </c>
@@ -7487,7 +7487,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>9</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>9</v>
       </c>
@@ -7545,7 +7545,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>9</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>14</v>
       </c>
@@ -7603,7 +7603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
         <v>40</v>
       </c>
@@ -7635,7 +7635,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
         <v>2172</v>
       </c>
@@ -7664,7 +7664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="34" t="s">
         <v>2173</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>97</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
         <v>94</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
         <v>100</v>
       </c>
@@ -7768,7 +7768,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
         <v>24</v>
       </c>
@@ -7797,7 +7797,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
         <v>41</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
         <v>88</v>
       </c>
@@ -7855,7 +7855,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>72</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
         <v>72</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
         <v>40</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="33" t="s">
         <v>88</v>
       </c>
@@ -7938,7 +7938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="33" t="s">
         <v>14</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
         <v>14</v>
       </c>
@@ -7972,7 +7972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="34" t="s">
         <v>14</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
         <v>83</v>
       </c>
@@ -8012,7 +8012,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="35" t="s">
         <v>40</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
         <v>83</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
         <v>41</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="s">
         <v>46</v>
       </c>
@@ -8086,7 +8086,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="33" t="s">
         <v>46</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="33" t="s">
         <v>24</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
         <v>83</v>
       </c>
@@ -8137,7 +8137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="34" t="s">
         <v>40</v>
       </c>
@@ -8154,7 +8154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="33" t="s">
         <v>72</v>
       </c>
@@ -8171,7 +8171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="33" t="s">
         <v>72</v>
       </c>
@@ -8188,7 +8188,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="34" t="s">
         <v>2173</v>
       </c>
@@ -8205,7 +8205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="34" t="s">
         <v>2173</v>
       </c>
@@ -8222,7 +8222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="34" t="s">
         <v>2173</v>
       </c>
@@ -8239,7 +8239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="34" t="s">
         <v>2173</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="34" t="s">
         <v>2170</v>
       </c>
@@ -8276,7 +8276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="34" t="s">
         <v>2171</v>
       </c>
@@ -8293,7 +8293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="33" t="s">
         <v>72</v>
       </c>
@@ -8310,7 +8310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="34" t="s">
         <v>2173</v>
       </c>
@@ -8327,7 +8327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="33" t="s">
         <v>83</v>
       </c>
@@ -8344,7 +8344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="34" t="s">
         <v>1025</v>
       </c>
@@ -8364,7 +8364,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="34" t="s">
         <v>993</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="34" t="s">
         <v>115</v>
       </c>
@@ -8398,7 +8398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="34" t="s">
         <v>40</v>
       </c>
@@ -8415,7 +8415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="33" t="s">
         <v>70</v>
       </c>
@@ -8432,7 +8432,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
         <v>72</v>
       </c>
@@ -8470,20 +8470,20 @@
   </sheetPr>
   <dimension ref="A1:N231"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A214" workbookViewId="0">
       <selection activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="10" max="10" width="46" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
         <v>121</v>
       </c>
@@ -8527,7 +8527,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
         <v>1027</v>
       </c>
@@ -8571,7 +8571,7 @@
         <v>30566</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="53" t="s">
         <v>1030</v>
       </c>
@@ -8615,7 +8615,7 @@
         <v>29985</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="53" t="s">
         <v>1036</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>27649</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="53" t="s">
         <v>1042</v>
       </c>
@@ -8703,7 +8703,7 @@
         <v>27803</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="53" t="s">
         <v>1047</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>30033</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="53" t="s">
         <v>1050</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>31890</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="53" t="s">
         <v>1054</v>
       </c>
@@ -8835,7 +8835,7 @@
         <v>30022</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="53" t="s">
         <v>1060</v>
       </c>
@@ -8879,7 +8879,7 @@
         <v>31363</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="53" t="s">
         <v>1063</v>
       </c>
@@ -8923,7 +8923,7 @@
         <v>30638</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="53" t="s">
         <v>1068</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>29441</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="53" t="s">
         <v>1072</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>30004</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="53" t="s">
         <v>1075</v>
       </c>
@@ -9055,7 +9055,7 @@
         <v>28487</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="53" t="s">
         <v>1080</v>
       </c>
@@ -9099,7 +9099,7 @@
         <v>29721</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="53" t="s">
         <v>1086</v>
       </c>
@@ -9143,7 +9143,7 @@
         <v>27831</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="53" t="s">
         <v>1094</v>
       </c>
@@ -9187,7 +9187,7 @@
         <v>28307</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="53" t="s">
         <v>1097</v>
       </c>
@@ -9231,7 +9231,7 @@
         <v>27453</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="53" t="s">
         <v>1103</v>
       </c>
@@ -9275,7 +9275,7 @@
         <v>29413</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="53" t="s">
         <v>1108</v>
       </c>
@@ -9319,7 +9319,7 @@
         <v>28671</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="53" t="s">
         <v>1114</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>28415</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="53" t="s">
         <v>1120</v>
       </c>
@@ -9407,7 +9407,7 @@
         <v>28306</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="53" t="s">
         <v>1127</v>
       </c>
@@ -9451,7 +9451,7 @@
         <v>31600</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="53" t="s">
         <v>1132</v>
       </c>
@@ -9495,7 +9495,7 @@
         <v>27649</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="53" t="s">
         <v>1138</v>
       </c>
@@ -9539,7 +9539,7 @@
         <v>29251</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="53" t="s">
         <v>1144</v>
       </c>
@@ -9583,7 +9583,7 @@
         <v>30721</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="53" t="s">
         <v>1150</v>
       </c>
@@ -9627,7 +9627,7 @@
         <v>27865</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="53" t="s">
         <v>1156</v>
       </c>
@@ -9671,7 +9671,7 @@
         <v>30270</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="53" t="s">
         <v>1158</v>
       </c>
@@ -9715,7 +9715,7 @@
         <v>30385</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="53" t="s">
         <v>1164</v>
       </c>
@@ -9759,7 +9759,7 @@
         <v>29292</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="53" t="s">
         <v>1170</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>30497</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="53" t="s">
         <v>1174</v>
       </c>
@@ -9847,7 +9847,7 @@
         <v>31176</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="53" t="s">
         <v>1177</v>
       </c>
@@ -9889,7 +9889,7 @@
       </c>
       <c r="N32" s="56"/>
     </row>
-    <row r="33" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="53" t="s">
         <v>1179</v>
       </c>
@@ -9933,7 +9933,7 @@
         <v>28109</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="53" t="s">
         <v>1184</v>
       </c>
@@ -9977,7 +9977,7 @@
         <v>27992</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="53" t="s">
         <v>1190</v>
       </c>
@@ -10021,7 +10021,7 @@
         <v>31721</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="53" t="s">
         <v>1192</v>
       </c>
@@ -10065,7 +10065,7 @@
         <v>28095</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="53" t="s">
         <v>1195</v>
       </c>
@@ -10109,7 +10109,7 @@
         <v>30610</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="53" t="s">
         <v>1200</v>
       </c>
@@ -10153,7 +10153,7 @@
         <v>30347</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="53" t="s">
         <v>1203</v>
       </c>
@@ -10197,7 +10197,7 @@
         <v>30888</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="53" t="s">
         <v>1206</v>
       </c>
@@ -10241,7 +10241,7 @@
         <v>30894</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="53" t="s">
         <v>1209</v>
       </c>
@@ -10285,7 +10285,7 @@
         <v>31526</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="53" t="s">
         <v>1216</v>
       </c>
@@ -10329,7 +10329,7 @@
         <v>27453</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="53" t="s">
         <v>1219</v>
       </c>
@@ -10373,7 +10373,7 @@
         <v>30117</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="53" t="s">
         <v>1222</v>
       </c>
@@ -10417,7 +10417,7 @@
         <v>29028</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="53" t="s">
         <v>1228</v>
       </c>
@@ -10461,7 +10461,7 @@
         <v>27957</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="53" t="s">
         <v>1234</v>
       </c>
@@ -10505,7 +10505,7 @@
         <v>31541</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="53" t="s">
         <v>1240</v>
       </c>
@@ -10549,7 +10549,7 @@
         <v>32226</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="53" t="s">
         <v>1245</v>
       </c>
@@ -10593,7 +10593,7 @@
         <v>29795</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="53" t="s">
         <v>1248</v>
       </c>
@@ -10637,7 +10637,7 @@
         <v>29875</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="53" t="s">
         <v>1254</v>
       </c>
@@ -10681,7 +10681,7 @@
         <v>27831</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="53" t="s">
         <v>1260</v>
       </c>
@@ -10725,7 +10725,7 @@
         <v>28272</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="53" t="s">
         <v>1264</v>
       </c>
@@ -10769,7 +10769,7 @@
         <v>29112</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="53" t="s">
         <v>1270</v>
       </c>
@@ -10813,7 +10813,7 @@
         <v>31441</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="53" t="s">
         <v>1273</v>
       </c>
@@ -10857,7 +10857,7 @@
         <v>27492</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="53" t="s">
         <v>1279</v>
       </c>
@@ -10901,7 +10901,7 @@
         <v>28794</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="53" t="s">
         <v>1284</v>
       </c>
@@ -10945,7 +10945,7 @@
         <v>27831</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="53" t="s">
         <v>1291</v>
       </c>
@@ -10989,7 +10989,7 @@
         <v>27453</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="53" t="s">
         <v>1296</v>
       </c>
@@ -11033,7 +11033,7 @@
         <v>27619</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="53" t="s">
         <v>1301</v>
       </c>
@@ -11077,7 +11077,7 @@
         <v>30013</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="53" t="s">
         <v>1304</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>31944</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="53" t="s">
         <v>1308</v>
       </c>
@@ -11165,7 +11165,7 @@
         <v>29699</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="53" t="s">
         <v>1313</v>
       </c>
@@ -11209,7 +11209,7 @@
         <v>28146</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="53" t="s">
         <v>1318</v>
       </c>
@@ -11253,7 +11253,7 @@
         <v>29699</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="53" t="s">
         <v>1324</v>
       </c>
@@ -11297,7 +11297,7 @@
         <v>30582</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="53" t="s">
         <v>1331</v>
       </c>
@@ -11341,7 +11341,7 @@
         <v>31376</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="53" t="s">
         <v>1334</v>
       </c>
@@ -11385,7 +11385,7 @@
         <v>31685</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="53" t="s">
         <v>1337</v>
       </c>
@@ -11429,7 +11429,7 @@
         <v>28650</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="53" t="s">
         <v>1343</v>
       </c>
@@ -11473,7 +11473,7 @@
         <v>30726</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="53" t="s">
         <v>1346</v>
       </c>
@@ -11517,7 +11517,7 @@
         <v>30508</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="53" t="s">
         <v>1351</v>
       </c>
@@ -11561,7 +11561,7 @@
         <v>31603</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="53" t="s">
         <v>1356</v>
       </c>
@@ -11605,7 +11605,7 @@
         <v>33557</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="53" t="s">
         <v>1358</v>
       </c>
@@ -11649,7 +11649,7 @@
         <v>28671</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="53" t="s">
         <v>1363</v>
       </c>
@@ -11693,7 +11693,7 @@
         <v>30025</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="53" t="s">
         <v>1368</v>
       </c>
@@ -11737,7 +11737,7 @@
         <v>32181</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="53" t="s">
         <v>1370</v>
       </c>
@@ -11781,7 +11781,7 @@
         <v>27572</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="53" t="s">
         <v>1375</v>
       </c>
@@ -11825,7 +11825,7 @@
         <v>27703</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="53" t="s">
         <v>1379</v>
       </c>
@@ -11869,7 +11869,7 @@
         <v>27733</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="53" t="s">
         <v>1382</v>
       </c>
@@ -11913,7 +11913,7 @@
         <v>28160</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="53" t="s">
         <v>1385</v>
       </c>
@@ -11957,7 +11957,7 @@
         <v>29094</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="53" t="s">
         <v>1388</v>
       </c>
@@ -12001,7 +12001,7 @@
         <v>29479</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="53" t="s">
         <v>1392</v>
       </c>
@@ -12045,7 +12045,7 @@
         <v>30043</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="53" t="s">
         <v>1395</v>
       </c>
@@ -12089,7 +12089,7 @@
         <v>31469</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="53" t="s">
         <v>1399</v>
       </c>
@@ -12133,7 +12133,7 @@
         <v>31581</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="53" t="s">
         <v>1403</v>
       </c>
@@ -12177,7 +12177,7 @@
         <v>29802</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="53" t="s">
         <v>1409</v>
       </c>
@@ -12221,7 +12221,7 @@
         <v>27886</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="53" t="s">
         <v>1415</v>
       </c>
@@ -12265,7 +12265,7 @@
         <v>29543</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="53" t="s">
         <v>1418</v>
       </c>
@@ -12309,7 +12309,7 @@
         <v>30162</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="53" t="s">
         <v>1424</v>
       </c>
@@ -12353,7 +12353,7 @@
         <v>30270</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="53" t="s">
         <v>1428</v>
       </c>
@@ -12397,7 +12397,7 @@
         <v>30792</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="53" t="s">
         <v>1434</v>
       </c>
@@ -12441,7 +12441,7 @@
         <v>31835</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="53" t="s">
         <v>1436</v>
       </c>
@@ -12485,7 +12485,7 @@
         <v>27841</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="53" t="s">
         <v>1439</v>
       </c>
@@ -12529,7 +12529,7 @@
         <v>28478</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="53" t="s">
         <v>1443</v>
       </c>
@@ -12573,7 +12573,7 @@
         <v>29875</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="53" t="s">
         <v>1451</v>
       </c>
@@ -12617,7 +12617,7 @@
         <v>31414</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="53" t="s">
         <v>1454</v>
       </c>
@@ -12661,7 +12661,7 @@
         <v>32051</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="53" t="s">
         <v>1457</v>
       </c>
@@ -12705,7 +12705,7 @@
         <v>27551</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="53" t="s">
         <v>1463</v>
       </c>
@@ -12749,7 +12749,7 @@
         <v>30106</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="53" t="s">
         <v>1465</v>
       </c>
@@ -12793,7 +12793,7 @@
         <v>29875</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="53" t="s">
         <v>1471</v>
       </c>
@@ -12837,7 +12837,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="53" t="s">
         <v>1478</v>
       </c>
@@ -12881,7 +12881,7 @@
         <v>29327</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="53" t="s">
         <v>1487</v>
       </c>
@@ -12925,7 +12925,7 @@
         <v>28153</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="53" t="s">
         <v>1493</v>
       </c>
@@ -12969,7 +12969,7 @@
         <v>30293</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="53" t="s">
         <v>1499</v>
       </c>
@@ -13013,7 +13013,7 @@
         <v>27606</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="53" t="s">
         <v>1505</v>
       </c>
@@ -13057,7 +13057,7 @@
         <v>30305</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="53" t="s">
         <v>1509</v>
       </c>
@@ -13101,7 +13101,7 @@
         <v>30470</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="53" t="s">
         <v>1512</v>
       </c>
@@ -13145,7 +13145,7 @@
         <v>31411</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="53" t="s">
         <v>1517</v>
       </c>
@@ -13189,7 +13189,7 @@
         <v>31649</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="53" t="s">
         <v>1519</v>
       </c>
@@ -13233,7 +13233,7 @@
         <v>29174</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="53" t="s">
         <v>1523</v>
       </c>
@@ -13277,7 +13277,7 @@
         <v>30131</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="53" t="s">
         <v>1528</v>
       </c>
@@ -13321,7 +13321,7 @@
         <v>30203</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="53" t="s">
         <v>1533</v>
       </c>
@@ -13365,7 +13365,7 @@
         <v>31453</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="53" t="s">
         <v>1535</v>
       </c>
@@ -13409,7 +13409,7 @@
         <v>29830</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="53" t="s">
         <v>1541</v>
       </c>
@@ -13453,7 +13453,7 @@
         <v>30441</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="53" t="s">
         <v>1544</v>
       </c>
@@ -13497,7 +13497,7 @@
         <v>30788</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="53" t="s">
         <v>1547</v>
       </c>
@@ -13541,7 +13541,7 @@
         <v>29210</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="53" t="s">
         <v>1554</v>
       </c>
@@ -13585,7 +13585,7 @@
         <v>32960</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="53" t="s">
         <v>1558</v>
       </c>
@@ -13629,7 +13629,7 @@
         <v>28626</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="53" t="s">
         <v>1564</v>
       </c>
@@ -13673,7 +13673,7 @@
         <v>31992</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="53" t="s">
         <v>1566</v>
       </c>
@@ -13717,7 +13717,7 @@
         <v>27999</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="53" t="s">
         <v>1573</v>
       </c>
@@ -13761,7 +13761,7 @@
         <v>30203</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="53" t="s">
         <v>1578</v>
       </c>
@@ -13805,7 +13805,7 @@
         <v>27523</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="53" t="s">
         <v>1584</v>
       </c>
@@ -13849,7 +13849,7 @@
         <v>31960</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="53" t="s">
         <v>1586</v>
       </c>
@@ -13893,7 +13893,7 @@
         <v>30295</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="53" t="s">
         <v>1592</v>
       </c>
@@ -13937,7 +13937,7 @@
         <v>28126</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="53" t="s">
         <v>1598</v>
       </c>
@@ -13981,7 +13981,7 @@
         <v>29350</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="53" t="s">
         <v>1602</v>
       </c>
@@ -14025,7 +14025,7 @@
         <v>31448</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="53" t="s">
         <v>1604</v>
       </c>
@@ -14069,7 +14069,7 @@
         <v>27886</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="53" t="s">
         <v>1611</v>
       </c>
@@ -14113,7 +14113,7 @@
         <v>28912</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="53" t="s">
         <v>1614</v>
       </c>
@@ -14157,7 +14157,7 @@
         <v>31146</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="53" t="s">
         <v>1620</v>
       </c>
@@ -14201,7 +14201,7 @@
         <v>29826</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="53" t="s">
         <v>1623</v>
       </c>
@@ -14245,7 +14245,7 @@
         <v>29082</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="53" t="s">
         <v>1628</v>
       </c>
@@ -14289,7 +14289,7 @@
         <v>30188</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="53" t="s">
         <v>1633</v>
       </c>
@@ -14333,7 +14333,7 @@
         <v>29845</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="53" t="s">
         <v>1636</v>
       </c>
@@ -14377,7 +14377,7 @@
         <v>31596</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="53" t="s">
         <v>1639</v>
       </c>
@@ -14421,7 +14421,7 @@
         <v>28605</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="53" t="s">
         <v>1645</v>
       </c>
@@ -14465,7 +14465,7 @@
         <v>31352</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="53" t="s">
         <v>1647</v>
       </c>
@@ -14509,7 +14509,7 @@
         <v>27528</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="53" t="s">
         <v>1653</v>
       </c>
@@ -14553,7 +14553,7 @@
         <v>30085</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="53" t="s">
         <v>1656</v>
       </c>
@@ -14597,7 +14597,7 @@
         <v>29795</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="53" t="s">
         <v>1659</v>
       </c>
@@ -14641,7 +14641,7 @@
         <v>31572</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="53" t="s">
         <v>1662</v>
       </c>
@@ -14685,7 +14685,7 @@
         <v>30371</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="53" t="s">
         <v>1668</v>
       </c>
@@ -14729,7 +14729,7 @@
         <v>29052</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="53" t="s">
         <v>1672</v>
       </c>
@@ -14773,7 +14773,7 @@
         <v>30294</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="53" t="s">
         <v>1676</v>
       </c>
@@ -14817,7 +14817,7 @@
         <v>28521</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="53" t="s">
         <v>1682</v>
       </c>
@@ -14861,7 +14861,7 @@
         <v>28174</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="53" t="s">
         <v>1687</v>
       </c>
@@ -14905,7 +14905,7 @@
         <v>30879</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="53" t="s">
         <v>1693</v>
       </c>
@@ -14949,7 +14949,7 @@
         <v>27485</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="53" t="s">
         <v>1698</v>
       </c>
@@ -14993,7 +14993,7 @@
         <v>27719</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="53" t="s">
         <v>1703</v>
       </c>
@@ -15037,7 +15037,7 @@
         <v>31061</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="53" t="s">
         <v>1706</v>
       </c>
@@ -15081,7 +15081,7 @@
         <v>31257</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="53" t="s">
         <v>1709</v>
       </c>
@@ -15125,7 +15125,7 @@
         <v>30229</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="53" t="s">
         <v>1716</v>
       </c>
@@ -15169,7 +15169,7 @@
         <v>30434</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="53" t="s">
         <v>1719</v>
       </c>
@@ -15211,7 +15211,7 @@
       </c>
       <c r="N153" s="56"/>
     </row>
-    <row r="154" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="53" t="s">
         <v>1722</v>
       </c>
@@ -15255,7 +15255,7 @@
         <v>29857</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="53" t="s">
         <v>1728</v>
       </c>
@@ -15299,7 +15299,7 @@
         <v>32307</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="53" t="s">
         <v>1731</v>
       </c>
@@ -15343,7 +15343,7 @@
         <v>27831</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="53" t="s">
         <v>1735</v>
       </c>
@@ -15387,7 +15387,7 @@
         <v>28993</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="53" t="s">
         <v>1741</v>
       </c>
@@ -15431,7 +15431,7 @@
         <v>29572</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="53" t="s">
         <v>1744</v>
       </c>
@@ -15475,7 +15475,7 @@
         <v>27845</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="53" t="s">
         <v>1751</v>
       </c>
@@ -15519,7 +15519,7 @@
         <v>30007</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="53" t="s">
         <v>1753</v>
       </c>
@@ -15563,7 +15563,7 @@
         <v>31541</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="53" t="s">
         <v>1755</v>
       </c>
@@ -15607,7 +15607,7 @@
         <v>32493</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="53" t="s">
         <v>1758</v>
       </c>
@@ -15651,7 +15651,7 @@
         <v>31215</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="53" t="s">
         <v>1763</v>
       </c>
@@ -15695,7 +15695,7 @@
         <v>29959</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="53" t="s">
         <v>1769</v>
       </c>
@@ -15739,7 +15739,7 @@
         <v>28230</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="53" t="s">
         <v>1776</v>
       </c>
@@ -15783,7 +15783,7 @@
         <v>27649</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="53" t="s">
         <v>1782</v>
       </c>
@@ -15827,7 +15827,7 @@
         <v>30229</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="53" t="s">
         <v>1787</v>
       </c>
@@ -15871,7 +15871,7 @@
         <v>31411</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="53" t="s">
         <v>1790</v>
       </c>
@@ -15915,7 +15915,7 @@
         <v>27971</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="53" t="s">
         <v>1793</v>
       </c>
@@ -15959,7 +15959,7 @@
         <v>32057</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="53" t="s">
         <v>1795</v>
       </c>
@@ -16003,7 +16003,7 @@
         <v>27572</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="53" t="s">
         <v>1798</v>
       </c>
@@ -16047,7 +16047,7 @@
         <v>30291</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="53" t="s">
         <v>1802</v>
       </c>
@@ -16091,7 +16091,7 @@
         <v>31301</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="53" t="s">
         <v>1807</v>
       </c>
@@ -16135,7 +16135,7 @@
         <v>27551</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="53" t="s">
         <v>1813</v>
       </c>
@@ -16179,7 +16179,7 @@
         <v>31691</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="53" t="s">
         <v>1816</v>
       </c>
@@ -16223,7 +16223,7 @@
         <v>34515</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="53" t="s">
         <v>1821</v>
       </c>
@@ -16267,7 +16267,7 @@
         <v>28531</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="53" t="s">
         <v>1827</v>
       </c>
@@ -16311,7 +16311,7 @@
         <v>29675</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="53" t="s">
         <v>1832</v>
       </c>
@@ -16355,7 +16355,7 @@
         <v>27845</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="53" t="s">
         <v>1838</v>
       </c>
@@ -16399,7 +16399,7 @@
         <v>31243</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="53" t="s">
         <v>1841</v>
       </c>
@@ -16443,7 +16443,7 @@
         <v>29263</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="53" t="s">
         <v>1847</v>
       </c>
@@ -16487,7 +16487,7 @@
         <v>28615</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="53" t="s">
         <v>1853</v>
       </c>
@@ -16531,7 +16531,7 @@
         <v>27971</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="53" t="s">
         <v>1859</v>
       </c>
@@ -16575,7 +16575,7 @@
         <v>28307</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="53" t="s">
         <v>1862</v>
       </c>
@@ -16619,7 +16619,7 @@
         <v>31859</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="53" t="s">
         <v>1868</v>
       </c>
@@ -16663,7 +16663,7 @@
         <v>30256</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="53" t="s">
         <v>1873</v>
       </c>
@@ -16707,7 +16707,7 @@
         <v>32104</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="53" t="s">
         <v>1875</v>
       </c>
@@ -16751,7 +16751,7 @@
         <v>29921</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="53" t="s">
         <v>1880</v>
       </c>
@@ -16795,7 +16795,7 @@
         <v>31691</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="53" t="s">
         <v>1882</v>
       </c>
@@ -16839,7 +16839,7 @@
         <v>30760</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="53" t="s">
         <v>1889</v>
       </c>
@@ -16883,7 +16883,7 @@
         <v>31635</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="53" t="s">
         <v>1892</v>
       </c>
@@ -16927,7 +16927,7 @@
         <v>32321</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="53" t="s">
         <v>1894</v>
       </c>
@@ -16971,7 +16971,7 @@
         <v>30229</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="53" t="s">
         <v>1899</v>
       </c>
@@ -17015,7 +17015,7 @@
         <v>30561</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="53" t="s">
         <v>1904</v>
       </c>
@@ -17059,7 +17059,7 @@
         <v>29182</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="53" t="s">
         <v>1910</v>
       </c>
@@ -17103,7 +17103,7 @@
         <v>28611</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="53" t="s">
         <v>1915</v>
       </c>
@@ -17147,7 +17147,7 @@
         <v>28881</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="53" t="s">
         <v>1921</v>
       </c>
@@ -17191,7 +17191,7 @@
         <v>27528</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="53" t="s">
         <v>1927</v>
       </c>
@@ -17235,7 +17235,7 @@
         <v>29035</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="53" t="s">
         <v>1929</v>
       </c>
@@ -17279,7 +17279,7 @@
         <v>29755</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="53" t="s">
         <v>1932</v>
       </c>
@@ -17323,7 +17323,7 @@
         <v>27803</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="53" t="s">
         <v>1938</v>
       </c>
@@ -17367,7 +17367,7 @@
         <v>33288</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="53" t="s">
         <v>1940</v>
       </c>
@@ -17411,7 +17411,7 @@
         <v>27705</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="53" t="s">
         <v>1946</v>
       </c>
@@ -17455,7 +17455,7 @@
         <v>27947</v>
       </c>
     </row>
-    <row r="205" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="53" t="s">
         <v>1954</v>
       </c>
@@ -17499,7 +17499,7 @@
         <v>29278</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="53" t="s">
         <v>1957</v>
       </c>
@@ -17543,7 +17543,7 @@
         <v>29479</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="53" t="s">
         <v>1962</v>
       </c>
@@ -17587,7 +17587,7 @@
         <v>30519</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="53" t="s">
         <v>1965</v>
       </c>
@@ -17631,7 +17631,7 @@
         <v>27485</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="53" t="s">
         <v>1971</v>
       </c>
@@ -17675,7 +17675,7 @@
         <v>32274</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="53" t="s">
         <v>1973</v>
       </c>
@@ -17719,7 +17719,7 @@
         <v>27813</v>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="53" t="s">
         <v>1978</v>
       </c>
@@ -17763,7 +17763,7 @@
         <v>27803</v>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="53" t="s">
         <v>1983</v>
       </c>
@@ -17807,7 +17807,7 @@
         <v>29795</v>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="53" t="s">
         <v>1989</v>
       </c>
@@ -17851,7 +17851,7 @@
         <v>27593</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="53" t="s">
         <v>1995</v>
       </c>
@@ -17895,7 +17895,7 @@
         <v>31768</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="53" t="s">
         <v>2003</v>
       </c>
@@ -17939,7 +17939,7 @@
         <v>29292</v>
       </c>
     </row>
-    <row r="216" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="53" t="s">
         <v>2009</v>
       </c>
@@ -17983,7 +17983,7 @@
         <v>31667</v>
       </c>
     </row>
-    <row r="217" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="53" t="s">
         <v>2014</v>
       </c>
@@ -18027,7 +18027,7 @@
         <v>31506</v>
       </c>
     </row>
-    <row r="218" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="53" t="s">
         <v>2020</v>
       </c>
@@ -18071,7 +18071,7 @@
         <v>29174</v>
       </c>
     </row>
-    <row r="219" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="53" t="s">
         <v>2026</v>
       </c>
@@ -18115,7 +18115,7 @@
         <v>31352</v>
       </c>
     </row>
-    <row r="220" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="53" t="s">
         <v>2029</v>
       </c>
@@ -18159,7 +18159,7 @@
         <v>28095</v>
       </c>
     </row>
-    <row r="221" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="53" t="s">
         <v>2033</v>
       </c>
@@ -18203,7 +18203,7 @@
         <v>27901</v>
       </c>
     </row>
-    <row r="222" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="53" t="s">
         <v>2039</v>
       </c>
@@ -18247,7 +18247,7 @@
         <v>31126</v>
       </c>
     </row>
-    <row r="223" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="53" t="s">
         <v>2045</v>
       </c>
@@ -18291,7 +18291,7 @@
         <v>29830</v>
       </c>
     </row>
-    <row r="224" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="53" t="s">
         <v>2051</v>
       </c>
@@ -18335,7 +18335,7 @@
         <v>29479</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="53" t="s">
         <v>2055</v>
       </c>
@@ -18379,7 +18379,7 @@
         <v>30251</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="53" t="s">
         <v>2057</v>
       </c>
@@ -18423,7 +18423,7 @@
         <v>31105</v>
       </c>
     </row>
-    <row r="227" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="53" t="s">
         <v>2062</v>
       </c>
@@ -18467,7 +18467,7 @@
         <v>32321</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="53" t="s">
         <v>2065</v>
       </c>
@@ -18511,7 +18511,7 @@
         <v>27610</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="53" t="s">
         <v>2071</v>
       </c>
@@ -18555,7 +18555,7 @@
         <v>29642</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="53" t="s">
         <v>2077</v>
       </c>
@@ -18599,7 +18599,7 @@
         <v>31231</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="53" t="s">
         <v>2080</v>
       </c>
@@ -18659,16 +18659,16 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
         <v>121</v>
       </c>
@@ -18847,7 +18847,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="58" t="s">
         <v>2086</v>
       </c>
@@ -19012,7 +19012,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="58" t="s">
         <v>2091</v>
       </c>
@@ -19181,7 +19181,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="58" t="s">
         <v>2101</v>
       </c>
@@ -19346,7 +19346,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58" t="s">
         <v>2112</v>
       </c>
@@ -19515,7 +19515,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="58" t="s">
         <v>2117</v>
       </c>
@@ -19680,7 +19680,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="58" t="s">
         <v>2127</v>
       </c>
@@ -19858,16 +19858,16 @@
   <dimension ref="A1:BG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="62" t="s">
         <v>121</v>
       </c>
@@ -20046,7 +20046,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="63" t="s">
         <v>2135</v>
       </c>
@@ -20211,7 +20211,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="63" t="s">
         <v>2149</v>
       </c>
@@ -20372,7 +20372,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="63" t="s">
         <v>2154</v>
       </c>
@@ -20533,7 +20533,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="63" t="s">
         <v>2159</v>
       </c>
@@ -20696,7 +20696,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="63" t="s">
         <v>2163</v>
       </c>
@@ -20870,23 +20870,23 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>121</v>
       </c>
@@ -20927,7 +20927,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>134</v>
       </c>
@@ -20968,7 +20968,7 @@
         <v>32609</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>143</v>
       </c>
@@ -21009,7 +21009,7 @@
         <v>32521</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>150</v>
       </c>
@@ -21050,7 +21050,7 @@
         <v>32591</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>156</v>
       </c>
@@ -21091,7 +21091,7 @@
         <v>30799</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>163</v>
       </c>
@@ -21132,7 +21132,7 @@
         <v>32590</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>169</v>
       </c>
@@ -21189,17 +21189,17 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>121</v>
       </c>
@@ -21324,7 +21324,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:41" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>221</v>
       </c>
@@ -21435,7 +21435,7 @@
       <c r="AN2" s="13"/>
       <c r="AO2" s="13"/>
     </row>
-    <row r="3" spans="1:41" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>235</v>
       </c>
@@ -21564,18 +21564,18 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>121</v>
       </c>
@@ -21754,7 +21754,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>247</v>
       </c>
@@ -21919,7 +21919,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>260</v>
       </c>
@@ -22082,7 +22082,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>265</v>
       </c>
@@ -22247,7 +22247,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>278</v>
       </c>
@@ -22410,7 +22410,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>290</v>
       </c>
@@ -22573,7 +22573,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>299</v>
       </c>
@@ -22736,7 +22736,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>308</v>
       </c>
@@ -22899,7 +22899,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>317</v>
       </c>
@@ -23064,7 +23064,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>321</v>
       </c>
@@ -23229,7 +23229,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>329</v>
       </c>
@@ -23394,7 +23394,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>341</v>
       </c>
@@ -23559,7 +23559,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>351</v>
       </c>
@@ -23724,7 +23724,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>357</v>
       </c>
@@ -23889,7 +23889,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>364</v>
       </c>
@@ -24054,7 +24054,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>369</v>
       </c>
@@ -24219,7 +24219,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>380</v>
       </c>
@@ -24384,7 +24384,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>392</v>
       </c>
@@ -24547,7 +24547,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>402</v>
       </c>
@@ -24710,7 +24710,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>405</v>
       </c>
@@ -24875,7 +24875,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>414</v>
       </c>
@@ -25038,7 +25038,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>425</v>
       </c>
@@ -25201,7 +25201,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>434</v>
       </c>
@@ -25364,7 +25364,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>444</v>
       </c>
@@ -25527,7 +25527,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>456</v>
       </c>
@@ -25690,7 +25690,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>463</v>
       </c>
@@ -25853,7 +25853,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>474</v>
       </c>
@@ -26016,7 +26016,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>485</v>
       </c>
@@ -26181,7 +26181,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>495</v>
       </c>
@@ -26346,7 +26346,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="30" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>500</v>
       </c>
@@ -26509,7 +26509,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>510</v>
       </c>
@@ -26678,7 +26678,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="32" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>518</v>
       </c>
@@ -26841,7 +26841,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="33" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>525</v>
       </c>
@@ -27006,7 +27006,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
         <v>531</v>
       </c>
@@ -27171,7 +27171,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
         <v>538</v>
       </c>
@@ -27334,7 +27334,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>551</v>
       </c>
@@ -27497,7 +27497,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>561</v>
       </c>
@@ -27660,7 +27660,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="38" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>570</v>
       </c>
@@ -27825,7 +27825,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="39" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>580</v>
       </c>
@@ -27988,7 +27988,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="40" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>591</v>
       </c>
@@ -28151,7 +28151,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="41" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
         <v>600</v>
       </c>
@@ -28314,7 +28314,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="42" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
         <v>611</v>
       </c>
@@ -28477,7 +28477,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="43" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
         <v>616</v>
       </c>
@@ -28638,7 +28638,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
         <v>624</v>
       </c>
@@ -28801,7 +28801,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="45" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
         <v>635</v>
       </c>
@@ -28964,7 +28964,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>644</v>
       </c>
@@ -29127,7 +29127,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="47" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
         <v>651</v>
       </c>
@@ -29290,7 +29290,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
         <v>663</v>
       </c>
@@ -29457,7 +29457,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
         <v>674</v>
       </c>
@@ -29622,7 +29622,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="50" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
         <v>684</v>
       </c>
@@ -29787,7 +29787,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="51" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
         <v>694</v>
       </c>
@@ -29950,7 +29950,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="52" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15" t="s">
         <v>703</v>
       </c>
@@ -30113,7 +30113,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="53" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
         <v>712</v>
       </c>
@@ -30276,7 +30276,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="54" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="15" t="s">
         <v>717</v>
       </c>
@@ -30439,7 +30439,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="55" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
         <v>728</v>
       </c>
@@ -30602,7 +30602,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="56" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="15" t="s">
         <v>734</v>
       </c>
@@ -30784,18 +30784,18 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="24" max="24" width="14.42578125" customWidth="1"/>
+    <col min="24" max="24" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>121</v>
       </c>
@@ -30869,7 +30869,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>747</v>
       </c>
@@ -30939,7 +30939,7 @@
         <v>34703</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>755</v>
       </c>
@@ -31005,7 +31005,7 @@
       </c>
       <c r="X3" s="27"/>
     </row>
-    <row r="4" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>765</v>
       </c>
@@ -31071,7 +31071,7 @@
       </c>
       <c r="X4" s="27"/>
     </row>
-    <row r="5" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>775</v>
       </c>
@@ -31149,13 +31149,13 @@
   </sheetPr>
   <dimension ref="A1:BG12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.33203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>121</v>
       </c>
@@ -31334,7 +31334,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>784</v>
       </c>
@@ -31497,7 +31497,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>791</v>
       </c>
@@ -31660,7 +31660,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>845</v>
       </c>
@@ -31823,7 +31823,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>798</v>
       </c>
@@ -31986,7 +31986,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>806</v>
       </c>
@@ -32149,7 +32149,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>810</v>
       </c>
@@ -32312,7 +32312,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>822</v>
       </c>
@@ -32471,7 +32471,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>851</v>
       </c>
@@ -32634,7 +32634,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>833</v>
       </c>
@@ -32797,7 +32797,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>841</v>
       </c>
@@ -32960,7 +32960,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>857</v>
       </c>
@@ -33137,27 +33137,28 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" customWidth="1"/>
-    <col min="8" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="2.140625" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="23.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="5" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" customWidth="1"/>
+    <col min="11" max="11" width="4.109375" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="23.33203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>121</v>
       </c>
@@ -33201,7 +33202,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>871</v>
       </c>
@@ -33245,7 +33246,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
         <v>878</v>
       </c>
@@ -33289,7 +33290,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>884</v>
       </c>
@@ -33333,7 +33334,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>888</v>
       </c>
@@ -33377,7 +33378,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>893</v>
       </c>
@@ -33422,7 +33423,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>899</v>
       </c>
@@ -33466,7 +33467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
         <v>904</v>
       </c>
@@ -33513,7 +33514,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>911</v>
       </c>
@@ -33557,7 +33558,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
         <v>914</v>
       </c>
@@ -33601,7 +33602,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
         <v>919</v>
       </c>
@@ -33648,7 +33649,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="37" t="s">
         <v>925</v>
       </c>
@@ -33692,7 +33693,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>929</v>
       </c>
@@ -33736,7 +33737,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>933</v>
       </c>
@@ -33780,7 +33781,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>938</v>
       </c>
@@ -33824,7 +33825,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>944</v>
       </c>
@@ -33868,7 +33869,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>947</v>
       </c>
@@ -33912,7 +33913,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37" t="s">
         <v>953</v>
       </c>
@@ -33959,7 +33960,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>956</v>
       </c>
@@ -34006,7 +34007,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>960</v>
       </c>
@@ -34048,7 +34049,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>965</v>
       </c>
@@ -34090,7 +34091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>970</v>
       </c>
@@ -34135,7 +34136,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>976</v>
       </c>
@@ -34180,7 +34181,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="37" t="s">
         <v>980</v>
       </c>
@@ -34225,7 +34226,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37" t="s">
         <v>984</v>
       </c>
@@ -34284,23 +34285,23 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>121</v>
       </c>
@@ -34341,7 +34342,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>784</v>
       </c>
@@ -34382,7 +34383,7 @@
         <v>32413</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>791</v>
       </c>
@@ -34423,7 +34424,7 @@
         <v>32048</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>845</v>
       </c>
@@ -34464,7 +34465,7 @@
         <v>33784</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>1000</v>
       </c>
@@ -34505,7 +34506,7 @@
         <v>31695</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>798</v>
       </c>
@@ -34546,7 +34547,7 @@
         <v>31959</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>806</v>
       </c>
@@ -34587,7 +34588,7 @@
         <v>31838</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>810</v>
       </c>
@@ -34628,7 +34629,7 @@
         <v>32329</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>822</v>
       </c>
@@ -34667,7 +34668,7 @@
       </c>
       <c r="M9" s="50"/>
     </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>833</v>
       </c>
@@ -34708,7 +34709,7 @@
         <v>31671</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>841</v>
       </c>
@@ -34749,7 +34750,7 @@
         <v>31903</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="47" t="s">
         <v>1004</v>
       </c>
@@ -34801,21 +34802,21 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>121</v>
       </c>
@@ -34856,7 +34857,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>1010</v>
       </c>
@@ -34897,7 +34898,7 @@
         <v>31617</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>1012</v>
       </c>
@@ -34938,7 +34939,7 @@
         <v>29250</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>1015</v>
       </c>
@@ -34979,7 +34980,7 @@
         <v>36076</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>1019</v>
       </c>

</xml_diff>